<commit_message>
Added final submission of hw1
</commit_message>
<xml_diff>
--- a/hw1/assignment.xlsx
+++ b/hw1/assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/math3550/hw1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D720CD5E-F20A-D34B-A51F-2F18E9458898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF8F835-4134-A545-BCD2-6EA523EA6AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5040" yWindow="4320" windowWidth="31920" windowHeight="18920" xr2:uid="{78071D2A-C46F-4268-A79B-8CAAC95C3910}"/>
   </bookViews>
@@ -18,7 +18,9 @@
   </sheets>
   <definedNames>
     <definedName name="my_data">'LOAN CALCULATOR'!$B$14:$F$85</definedName>
-    <definedName name="my_data2">'LOAN CALCULATOR'!$B$14</definedName>
+    <definedName name="my_data2">'LOAN CALCULATOR'!$B$14:$B$85</definedName>
+    <definedName name="my_data3">'LOAN CALCULATOR'!$A$13</definedName>
+    <definedName name="my_data4">'LOAN CALCULATOR'!$B$13:$F$13</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -64,9 +66,6 @@
   </si>
   <si>
     <t>Monthly Payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Using the LOAN CALCULATOR with the inuts from #5 above, use VLOOKUP to answer the following questions. </t>
   </si>
   <si>
     <t xml:space="preserve">     Enter your formulas in the yellow cells.</t>
@@ -177,6 +176,9 @@
       </rPr>
       <t>Balance</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Using the LOAN CALCULATOR with the inputs from #5 above, use VLOOKUP to answer the following questions. </t>
   </si>
 </sst>
 </file>
@@ -510,7 +512,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -893,7 +895,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1084,17 +1086,17 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="29" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1104,7 +1106,7 @@
         <v>31.73009360200663</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
@@ -1113,25 +1115,25 @@
         <v>28888.250763342101</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B27" s="32">
-        <f>INDEX(my_data, 34, 5)</f>
+        <f>INDEX(my_data, MATCH(34, my_data2, 0), MATCH("Ending Balance", my_data4, 0))</f>
         <v>27511.645858881842</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B29" s="32">
-        <f ca="1">OFFSET(my_data2, 44, 4)</f>
+        <f ca="1">OFFSET(my_data3, MATCH(45, my_data2, 0), MATCH("Ending Balance", my_data4, 0))</f>
         <v>19815.611966978096</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
@@ -1140,12 +1142,12 @@
         <v>34998.211693201731</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1159,8 +1161,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:N373"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A32" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1182,7 +1184,7 @@
     <row r="1" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="16">
         <v>50000</v>
@@ -1191,18 +1193,18 @@
     <row r="3" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="4"/>
       <c r="F3" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="14">
         <v>3.0141345355425203E-2</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="12">
         <f>C4/12</f>
@@ -1214,13 +1216,13 @@
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="11">
         <v>72</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="10">
         <f>VLOOKUP(C6,$B$14:$F$85,5,0)</f>
@@ -1232,7 +1234,7 @@
     </row>
     <row r="8" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="8">
         <v>760</v>
@@ -1241,7 +1243,7 @@
     <row r="9" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="7">
         <f>C8*C6</f>
@@ -1250,7 +1252,7 @@
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="35"/>
       <c r="D12" s="35"/>
@@ -1259,19 +1261,19 @@
     </row>
     <row r="13" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">

</xml_diff>